<commit_message>
update relative paths in prep_palm_input_update.m
</commit_message>
<xml_diff>
--- a/code/df_full_left.xlsx
+++ b/code/df_full_left.xlsx
@@ -13,7 +13,1057 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1820">
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
   <si>
     <t>IV-doors</t>
   </si>
@@ -4545,214 +5595,214 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1400</v>
+        <v>1750</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1401</v>
+        <v>1751</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1402</v>
+        <v>1752</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1403</v>
+        <v>1753</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1404</v>
+        <v>1754</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1405</v>
+        <v>1755</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1406</v>
+        <v>1756</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1407</v>
+        <v>1757</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1408</v>
+        <v>1758</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1409</v>
+        <v>1759</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1410</v>
+        <v>1760</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1411</v>
+        <v>1761</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1412</v>
+        <v>1762</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1413</v>
+        <v>1763</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1414</v>
+        <v>1764</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1415</v>
+        <v>1765</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>1416</v>
+        <v>1766</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>1417</v>
+        <v>1767</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>1418</v>
+        <v>1768</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>1419</v>
+        <v>1769</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>1420</v>
+        <v>1770</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>1421</v>
+        <v>1771</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>1422</v>
+        <v>1772</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>1423</v>
+        <v>1773</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>1424</v>
+        <v>1774</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>1425</v>
+        <v>1775</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>1426</v>
+        <v>1776</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>1427</v>
+        <v>1777</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>1428</v>
+        <v>1778</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>1429</v>
+        <v>1779</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>1430</v>
+        <v>1780</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>1431</v>
+        <v>1781</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>1432</v>
+        <v>1782</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>1433</v>
+        <v>1783</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>1434</v>
+        <v>1784</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>1435</v>
+        <v>1785</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>1436</v>
+        <v>1786</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>1437</v>
+        <v>1787</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>1438</v>
+        <v>1788</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>1439</v>
+        <v>1789</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>1440</v>
+        <v>1790</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>1441</v>
+        <v>1791</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>1442</v>
+        <v>1792</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>1443</v>
+        <v>1793</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>1444</v>
+        <v>1794</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>1445</v>
+        <v>1795</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>1446</v>
+        <v>1796</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>1447</v>
+        <v>1797</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>1448</v>
+        <v>1798</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>1449</v>
+        <v>1799</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>1451</v>
+        <v>1801</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>1452</v>
+        <v>1802</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>1453</v>
+        <v>1803</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>1454</v>
+        <v>1804</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>1455</v>
+        <v>1805</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>1456</v>
+        <v>1806</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>1457</v>
+        <v>1807</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>1458</v>
+        <v>1808</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>1459</v>
+        <v>1809</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>1460</v>
+        <v>1810</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>1461</v>
+        <v>1811</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>1462</v>
+        <v>1812</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>1463</v>
+        <v>1813</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>1464</v>
+        <v>1814</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>1465</v>
+        <v>1815</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>1466</v>
+        <v>1816</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>1467</v>
+        <v>1817</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>1468</v>
+        <v>1818</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>1469</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
add data for palm
</commit_message>
<xml_diff>
--- a/code/df_full_left.xlsx
+++ b/code/df_full_left.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5917" uniqueCount="5917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6130" uniqueCount="6130">
   <si>
     <t>IV-doors</t>
   </si>
@@ -10096,6 +10096,645 @@
   </si>
   <si>
     <t>Subs</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
+  </si>
+  <si>
+    <t>Subs</t>
+  </si>
+  <si>
+    <t>IV-doors</t>
+  </si>
+  <si>
+    <t>IV-socialdoors</t>
+  </si>
+  <si>
+    <t>IV-ugdg</t>
+  </si>
+  <si>
+    <t>IV-mid</t>
+  </si>
+  <si>
+    <t>IV-sharedreward</t>
+  </si>
+  <si>
+    <t>V-doors</t>
+  </si>
+  <si>
+    <t>V-socialdoors</t>
+  </si>
+  <si>
+    <t>V-ugdg</t>
+  </si>
+  <si>
+    <t>V-mid</t>
+  </si>
+  <si>
+    <t>V-sharedreward</t>
+  </si>
+  <si>
+    <t>VI-doors</t>
+  </si>
+  <si>
+    <t>VI-socialdoors</t>
+  </si>
+  <si>
+    <t>VI-ugdg</t>
+  </si>
+  <si>
+    <t>VI-mid</t>
+  </si>
+  <si>
+    <t>VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-I-doors</t>
+  </si>
+  <si>
+    <t>Crus-I-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-I-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-I-mid</t>
+  </si>
+  <si>
+    <t>Crus-I-sharedreward</t>
+  </si>
+  <si>
+    <t>Crus-II-doors</t>
+  </si>
+  <si>
+    <t>Crus-II-socialdoors</t>
+  </si>
+  <si>
+    <t>Crus-II-ugdg</t>
+  </si>
+  <si>
+    <t>Crus-II-mid</t>
+  </si>
+  <si>
+    <t>Crus-II-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIa-doors</t>
+  </si>
+  <si>
+    <t>VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIa-mid</t>
+  </si>
+  <si>
+    <t>VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>VIIIb-doors</t>
+  </si>
+  <si>
+    <t>VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>VIIIb-mid</t>
+  </si>
+  <si>
+    <t>VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>IX-doors</t>
+  </si>
+  <si>
+    <t>IX-socialdoors</t>
+  </si>
+  <si>
+    <t>IX-ugdg</t>
+  </si>
+  <si>
+    <t>IX-mid</t>
+  </si>
+  <si>
+    <t>IX-sharedreward</t>
+  </si>
+  <si>
+    <t>X-doors</t>
+  </si>
+  <si>
+    <t>X-socialdoors</t>
+  </si>
+  <si>
+    <t>X-ugdg</t>
+  </si>
+  <si>
+    <t>X-mid</t>
+  </si>
+  <si>
+    <t>X-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VI-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VI-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VI-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VI-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIa-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-doors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-mid</t>
+  </si>
+  <si>
+    <t>Vermis-VIIIb-sharedreward</t>
+  </si>
+  <si>
+    <t>Vermis-IX-doors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-socialdoors</t>
+  </si>
+  <si>
+    <t>Vermis-IX-ugdg</t>
+  </si>
+  <si>
+    <t>Vermis-IX-mid</t>
+  </si>
+  <si>
+    <t>Vermis-IX-sharedreward</t>
   </si>
   <si>
     <t>Subs</t>
@@ -17887,217 +18526,217 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5846</v>
+        <v>6059</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>5847</v>
+        <v>6060</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5848</v>
+        <v>6061</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5849</v>
+        <v>6062</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5850</v>
+        <v>6063</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5851</v>
+        <v>6064</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>5852</v>
+        <v>6065</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>5853</v>
+        <v>6066</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>5854</v>
+        <v>6067</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>5855</v>
+        <v>6068</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>5856</v>
+        <v>6069</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>5857</v>
+        <v>6070</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>5858</v>
+        <v>6071</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>5859</v>
+        <v>6072</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>5860</v>
+        <v>6073</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>5861</v>
+        <v>6074</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>5862</v>
+        <v>6075</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>5863</v>
+        <v>6076</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>5864</v>
+        <v>6077</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>5865</v>
+        <v>6078</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>5866</v>
+        <v>6079</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>5867</v>
+        <v>6080</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>5868</v>
+        <v>6081</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>5869</v>
+        <v>6082</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>5870</v>
+        <v>6083</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>5871</v>
+        <v>6084</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>5872</v>
+        <v>6085</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>5873</v>
+        <v>6086</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>5874</v>
+        <v>6087</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>5875</v>
+        <v>6088</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>5876</v>
+        <v>6089</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>5877</v>
+        <v>6090</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>5878</v>
+        <v>6091</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>5879</v>
+        <v>6092</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>5880</v>
+        <v>6093</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>5881</v>
+        <v>6094</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>5882</v>
+        <v>6095</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>5883</v>
+        <v>6096</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>5884</v>
+        <v>6097</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>5885</v>
+        <v>6098</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>5886</v>
+        <v>6099</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>5887</v>
+        <v>6100</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>5888</v>
+        <v>6101</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>5889</v>
+        <v>6102</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>5890</v>
+        <v>6103</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>5891</v>
+        <v>6104</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>5892</v>
+        <v>6105</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>5893</v>
+        <v>6106</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>5894</v>
+        <v>6107</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>5895</v>
+        <v>6108</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>5896</v>
+        <v>6109</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>5897</v>
+        <v>6110</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>5898</v>
+        <v>6111</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>5899</v>
+        <v>6112</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>5900</v>
+        <v>6113</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>5901</v>
+        <v>6114</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>5902</v>
+        <v>6115</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>5903</v>
+        <v>6116</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>5904</v>
+        <v>6117</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>5905</v>
+        <v>6118</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>5906</v>
+        <v>6119</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>5907</v>
+        <v>6120</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>5908</v>
+        <v>6121</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>5909</v>
+        <v>6122</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>5910</v>
+        <v>6123</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>5911</v>
+        <v>6124</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>5912</v>
+        <v>6125</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>5913</v>
+        <v>6126</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>5914</v>
+        <v>6127</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>5915</v>
+        <v>6128</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>5916</v>
+        <v>6129</v>
       </c>
     </row>
     <row r="2">

</xml_diff>